<commit_message>
'Administrative' changed to 'Official stats'.
</commit_message>
<xml_diff>
--- a/data/TEMPO_SR_2019-08-13.xlsx
+++ b/data/TEMPO_SR_2019-08-13.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\TEMPOSR-A1953\TEMPO_syst-rev\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\TEMPOSR-A1953\TEMPO_syst-rev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4011" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4011" uniqueCount="1122">
   <si>
     <t>Theme</t>
   </si>
@@ -3872,6 +3872,9 @@
   </si>
   <si>
     <t>Li, M., Zhang, H., &amp; Chen, J. (2019). Fine-Grained Dynamic Population Mapping Method Based on Large-Scale Sparse Mobile Phone Data. 2019 20th IEEE International Conference on Mobile Data Management (MDM), 473–478. https://doi.org/10.1109/MDM.2019.00008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Official statistics </t>
   </si>
 </sst>
 </file>
@@ -4391,17 +4394,17 @@
     <xf numFmtId="165" fontId="11" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6051,7 +6054,7 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="125" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -6087,7 +6090,7 @@
       <c r="AB2" s="9"/>
     </row>
     <row r="3" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="123"/>
+      <c r="A3" s="125"/>
       <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
@@ -6121,7 +6124,7 @@
       <c r="AB3" s="9"/>
     </row>
     <row r="4" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="123"/>
+      <c r="A4" s="125"/>
       <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
@@ -6173,7 +6176,7 @@
       <c r="AMJ4"/>
     </row>
     <row r="5" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="123"/>
+      <c r="A5" s="125"/>
       <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
@@ -6213,7 +6216,7 @@
       <c r="AB5" s="9"/>
     </row>
     <row r="6" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="123"/>
+      <c r="A6" s="125"/>
       <c r="B6" s="6" t="s">
         <v>37</v>
       </c>
@@ -6247,7 +6250,7 @@
       <c r="AB6" s="9"/>
     </row>
     <row r="7" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="123"/>
+      <c r="A7" s="125"/>
       <c r="B7" s="6" t="s">
         <v>39</v>
       </c>
@@ -6290,7 +6293,7 @@
       <c r="Y7" s="9"/>
     </row>
     <row r="8" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="123"/>
+      <c r="A8" s="125"/>
       <c r="B8" s="6" t="s">
         <v>47</v>
       </c>
@@ -6362,7 +6365,7 @@
       <c r="AB9" s="9"/>
     </row>
     <row r="10" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="124" t="s">
+      <c r="A10" s="126" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -6398,7 +6401,7 @@
       <c r="AB10" s="9"/>
     </row>
     <row r="11" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="11" t="s">
         <v>56</v>
       </c>
@@ -6434,7 +6437,7 @@
       <c r="AB11" s="9"/>
     </row>
     <row r="12" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="124"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="11" t="s">
         <v>59</v>
       </c>
@@ -6472,7 +6475,7 @@
       <c r="AB12" s="9"/>
     </row>
     <row r="13" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="124"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="11" t="s">
         <v>61</v>
       </c>
@@ -6514,7 +6517,7 @@
       <c r="AB13" s="12"/>
     </row>
     <row r="14" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="11" t="s">
         <v>67</v>
       </c>
@@ -6548,7 +6551,7 @@
       <c r="AB14" s="9"/>
     </row>
     <row r="15" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="124"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="11" t="s">
         <v>69</v>
       </c>
@@ -6582,7 +6585,7 @@
       <c r="AB15" s="9"/>
     </row>
     <row r="16" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="124"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="11" t="s">
         <v>71</v>
       </c>
@@ -6616,7 +6619,7 @@
       <c r="AB16" s="9"/>
     </row>
     <row r="17" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="124"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="11" t="s">
         <v>73</v>
       </c>
@@ -6650,7 +6653,7 @@
       <c r="AB17" s="9"/>
     </row>
     <row r="18" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="124"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="11" t="s">
         <v>75</v>
       </c>
@@ -6684,7 +6687,7 @@
       <c r="AB18" s="9"/>
     </row>
     <row r="19" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="124"/>
+      <c r="A19" s="126"/>
       <c r="B19" s="11" t="s">
         <v>77</v>
       </c>
@@ -6718,7 +6721,7 @@
       <c r="AB19" s="9"/>
     </row>
     <row r="20" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="124"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="11" t="s">
         <v>79</v>
       </c>
@@ -6752,7 +6755,7 @@
       <c r="AB20" s="9"/>
     </row>
     <row r="21" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="124"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="11" t="s">
         <v>81</v>
       </c>
@@ -6786,7 +6789,7 @@
       <c r="AB21" s="9"/>
     </row>
     <row r="22" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="124"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="11" t="s">
         <v>83</v>
       </c>
@@ -6824,7 +6827,7 @@
       <c r="AB22" s="9"/>
     </row>
     <row r="23" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="124"/>
+      <c r="A23" s="126"/>
       <c r="B23" s="11" t="s">
         <v>85</v>
       </c>
@@ -6862,7 +6865,7 @@
       <c r="AB23" s="9"/>
     </row>
     <row r="24" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="124"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="11" t="s">
         <v>87</v>
       </c>
@@ -6896,7 +6899,7 @@
       <c r="AB24" s="9"/>
     </row>
     <row r="25" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="124"/>
+      <c r="A25" s="126"/>
       <c r="B25" s="11" t="s">
         <v>89</v>
       </c>
@@ -6930,7 +6933,7 @@
       <c r="AB25" s="9"/>
     </row>
     <row r="26" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="124"/>
+      <c r="A26" s="126"/>
       <c r="B26" s="11" t="s">
         <v>91</v>
       </c>
@@ -6964,7 +6967,7 @@
       <c r="AB26" s="9"/>
     </row>
     <row r="27" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="124"/>
+      <c r="A27" s="126"/>
       <c r="B27" s="11" t="s">
         <v>93</v>
       </c>
@@ -7006,7 +7009,7 @@
       <c r="AB27" s="9"/>
     </row>
     <row r="28" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="124"/>
+      <c r="A28" s="126"/>
       <c r="B28" s="11" t="s">
         <v>99</v>
       </c>
@@ -7042,7 +7045,7 @@
       <c r="AB28" s="9"/>
     </row>
     <row r="29" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="124"/>
+      <c r="A29" s="126"/>
       <c r="B29" s="11" t="s">
         <v>102</v>
       </c>
@@ -7076,7 +7079,7 @@
       <c r="AB29" s="9"/>
     </row>
     <row r="30" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="124"/>
+      <c r="A30" s="126"/>
       <c r="B30" s="11" t="s">
         <v>104</v>
       </c>
@@ -7110,7 +7113,7 @@
       <c r="AB30" s="9"/>
     </row>
     <row r="31" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="124"/>
+      <c r="A31" s="126"/>
       <c r="B31" s="11" t="s">
         <v>106</v>
       </c>
@@ -7144,7 +7147,7 @@
       <c r="AB31" s="9"/>
     </row>
     <row r="32" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="124"/>
+      <c r="A32" s="126"/>
       <c r="B32" s="11" t="s">
         <v>108</v>
       </c>
@@ -7182,7 +7185,7 @@
       <c r="AB32" s="9"/>
     </row>
     <row r="33" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="124"/>
+      <c r="A33" s="126"/>
       <c r="B33" s="11" t="s">
         <v>110</v>
       </c>
@@ -7216,7 +7219,7 @@
       <c r="AB33" s="9"/>
     </row>
     <row r="34" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="124"/>
+      <c r="A34" s="126"/>
       <c r="B34" s="11" t="s">
         <v>112</v>
       </c>
@@ -7250,7 +7253,7 @@
       <c r="AB34" s="9"/>
     </row>
     <row r="35" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="124"/>
+      <c r="A35" s="126"/>
       <c r="B35" s="11" t="s">
         <v>114</v>
       </c>
@@ -8256,10 +8259,10 @@
   <dimension ref="A1:AMJ97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B86" sqref="B86"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -8599,14 +8602,14 @@
       </c>
     </row>
     <row r="2" spans="1:96" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="123" t="s">
         <v>190</v>
       </c>
       <c r="B2" s="26">
         <v>1925</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -8765,7 +8768,7 @@
       <c r="CR2" s="25"/>
     </row>
     <row r="3" spans="1:96" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="123" t="s">
         <v>197</v>
       </c>
       <c r="B3" s="26">
@@ -8946,7 +8949,7 @@
         <v>1068</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="F4" s="34"/>
       <c r="G4" s="34" t="s">
@@ -9288,7 +9291,7 @@
         <v>1951</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>1070</v>
@@ -10146,7 +10149,7 @@
         <v>1956</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>1068</v>
@@ -10335,7 +10338,7 @@
         <v>1068</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -10679,14 +10682,14 @@
       <c r="CR13" s="34"/>
     </row>
     <row r="14" spans="1:96" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="124" t="s">
         <v>271</v>
       </c>
       <c r="B14" s="48">
         <v>1968</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D14" s="47" t="s">
         <v>1068</v>
@@ -11040,7 +11043,7 @@
         <v>1984</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
@@ -11212,7 +11215,7 @@
         <v>1984</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
@@ -11386,7 +11389,7 @@
         <v>1990</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>1068</v>
@@ -11565,7 +11568,7 @@
       <c r="CR18" s="34"/>
     </row>
     <row r="19" spans="1:96" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="126" t="s">
+      <c r="A19" s="124" t="s">
         <v>311</v>
       </c>
       <c r="B19" s="48">
@@ -11731,14 +11734,14 @@
       <c r="CR19" s="34"/>
     </row>
     <row r="20" spans="1:96" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="126" t="s">
+      <c r="A20" s="124" t="s">
         <v>318</v>
       </c>
       <c r="B20" s="48">
         <v>1992</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D20" s="47" t="s">
         <v>1068</v>
@@ -12086,7 +12089,7 @@
         <v>1995</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
@@ -12452,7 +12455,7 @@
         <v>1998</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D24" s="34"/>
       <c r="E24" s="34"/>
@@ -12810,7 +12813,7 @@
         <v>1998</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
@@ -12979,7 +12982,7 @@
       <c r="CR26" s="34"/>
     </row>
     <row r="27" spans="1:96" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="126" t="s">
+      <c r="A27" s="124" t="s">
         <v>363</v>
       </c>
       <c r="B27" s="48">
@@ -13121,7 +13124,7 @@
       <c r="CR27" s="34"/>
     </row>
     <row r="28" spans="1:96" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="126" t="s">
+      <c r="A28" s="124" t="s">
         <v>367</v>
       </c>
       <c r="B28" s="48">
@@ -13131,7 +13134,7 @@
         <v>1070</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>1068</v>
@@ -13654,7 +13657,7 @@
         <v>2003</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D31" s="34" t="s">
         <v>1070</v>
@@ -13834,7 +13837,7 @@
         <v>2005</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
@@ -14030,7 +14033,7 @@
         <v>2006</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D33" s="34"/>
       <c r="E33" s="34"/>
@@ -14204,7 +14207,7 @@
         <v>2007</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D34" s="34" t="s">
         <v>1069</v>
@@ -14402,7 +14405,7 @@
         <v>2007</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D35" s="34"/>
       <c r="E35" s="34"/>
@@ -14778,7 +14781,7 @@
         <v>2007</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D37" s="34"/>
       <c r="E37" s="34"/>
@@ -14961,7 +14964,7 @@
         <v>1072</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="E38" s="34"/>
       <c r="F38" s="34"/>
@@ -15486,7 +15489,7 @@
         <v>2010</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D41" s="34" t="s">
         <v>1068</v>
@@ -15670,7 +15673,7 @@
         <v>2010</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D42" s="34" t="s">
         <v>1069</v>
@@ -16210,7 +16213,7 @@
         <v>2011</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D45" s="34"/>
       <c r="E45" s="34"/>
@@ -16583,7 +16586,7 @@
         <v>1068</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="E47" s="34"/>
       <c r="F47" s="34"/>
@@ -16758,7 +16761,7 @@
         <v>2011</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D48" s="34"/>
       <c r="E48" s="34"/>
@@ -17123,14 +17126,14 @@
       <c r="CR49" s="34"/>
     </row>
     <row r="50" spans="1:96" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="126" t="s">
+      <c r="A50" s="124" t="s">
         <v>570</v>
       </c>
       <c r="B50" s="48">
         <v>2011</v>
       </c>
       <c r="C50" s="47" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D50" s="47" t="s">
         <v>1068</v>
@@ -17286,7 +17289,7 @@
         <v>2012</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D51" s="34" t="s">
         <v>1068</v>
@@ -17657,7 +17660,7 @@
         <v>1068</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="E53" s="34"/>
       <c r="F53" s="34"/>
@@ -17824,7 +17827,7 @@
         <v>2013</v>
       </c>
       <c r="C54" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D54" s="34"/>
       <c r="E54" s="34"/>
@@ -17992,7 +17995,7 @@
         <v>2013</v>
       </c>
       <c r="C55" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D55" s="34" t="s">
         <v>1068</v>
@@ -18180,7 +18183,7 @@
         <v>2013</v>
       </c>
       <c r="C56" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D56" s="34"/>
       <c r="E56" s="34"/>
@@ -18514,7 +18517,7 @@
         <v>2014</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D58" s="34"/>
       <c r="E58" s="34"/>
@@ -19078,7 +19081,7 @@
         <v>2014</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D61" s="34"/>
       <c r="E61" s="34"/>
@@ -19274,7 +19277,7 @@
         <v>2014</v>
       </c>
       <c r="C62" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D62" s="34" t="s">
         <v>1068</v>
@@ -19462,7 +19465,7 @@
         <v>2014</v>
       </c>
       <c r="C63" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D63" s="34" t="s">
         <v>1068</v>
@@ -19646,7 +19649,7 @@
         <v>2015</v>
       </c>
       <c r="C64" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D64" s="34" t="s">
         <v>1069</v>
@@ -19822,7 +19825,7 @@
         <v>2015</v>
       </c>
       <c r="C65" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D65" s="34"/>
       <c r="E65" s="34"/>
@@ -20004,7 +20007,7 @@
         <v>2015</v>
       </c>
       <c r="C66" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D66" s="34"/>
       <c r="E66" s="34"/>
@@ -20184,7 +20187,7 @@
         <v>2015</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D67" s="34"/>
       <c r="E67" s="34"/>
@@ -20366,7 +20369,7 @@
         <v>2016</v>
       </c>
       <c r="C68" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D68" s="34"/>
       <c r="E68" s="34"/>
@@ -21844,7 +21847,7 @@
         <v>2016</v>
       </c>
       <c r="C71" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D71" s="34" t="s">
         <v>1071</v>
@@ -22402,7 +22405,7 @@
         <v>2017</v>
       </c>
       <c r="C74" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D74" s="34"/>
       <c r="E74" s="34"/>
@@ -22582,7 +22585,7 @@
         <v>2017</v>
       </c>
       <c r="C75" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D75" s="34"/>
       <c r="E75" s="34"/>
@@ -22964,7 +22967,7 @@
         <v>2017</v>
       </c>
       <c r="C77" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D77" s="34" t="s">
         <v>1068</v>
@@ -23142,7 +23145,7 @@
         <v>2017</v>
       </c>
       <c r="C78" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D78" s="34"/>
       <c r="E78" s="34"/>
@@ -23518,7 +23521,7 @@
         <v>1069</v>
       </c>
       <c r="D80" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="E80" s="34"/>
       <c r="F80" s="34"/>
@@ -23697,7 +23700,7 @@
         <v>2017</v>
       </c>
       <c r="C81" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D81" s="34"/>
       <c r="E81" s="34"/>
@@ -24421,7 +24424,7 @@
         <v>2018</v>
       </c>
       <c r="C85" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D85" s="34"/>
       <c r="E85" s="34"/>
@@ -24793,7 +24796,7 @@
         <v>2018</v>
       </c>
       <c r="C87" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D87" s="34" t="s">
         <v>1068</v>
@@ -25912,7 +25915,7 @@
         <v>28</v>
       </c>
       <c r="D93" s="106" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="E93" s="106" t="s">
         <v>1068</v>
@@ -26110,7 +26113,7 @@
         <v>2019</v>
       </c>
       <c r="C94" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="D94" s="34" t="s">
         <v>1069</v>
@@ -26317,7 +26320,7 @@
         <v>1068</v>
       </c>
       <c r="D95" s="34" t="s">
-        <v>1067</v>
+        <v>1121</v>
       </c>
       <c r="E95" s="34" t="s">
         <v>1070</v>

</xml_diff>

<commit_message>
All comments on board.
</commit_message>
<xml_diff>
--- a/data/TEMPO_SR_2019-08-13.xlsx
+++ b/data/TEMPO_SR_2019-08-13.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="5772" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="5772" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -7505,11 +7505,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C80" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
+      <selection pane="bottomRight" activeCell="BN1" sqref="BN1:BU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -26613,11 +26613,11 @@
   </sheetPr>
   <dimension ref="A1:AMK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="AW2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="BC2" sqref="BC2:BD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -26992,20 +26992,20 @@
       <c r="AX2" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="AY2" s="80"/>
-      <c r="AZ2" s="80"/>
+      <c r="AY2" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="AZ2" s="80" t="s">
+        <v>27</v>
+      </c>
       <c r="BA2" s="80" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BB2" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="BC2" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="BD2" s="80" t="s">
-        <v>27</v>
-      </c>
+      <c r="BC2" s="80"/>
+      <c r="BD2" s="80"/>
       <c r="BE2" s="80" t="s">
         <v>27</v>
       </c>

</xml_diff>